<commit_message>
new chamges 11 05
</commit_message>
<xml_diff>
--- a/schedule/Schedule_BA_SE_Sevik.xlsx
+++ b/schedule/Schedule_BA_SE_Sevik.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EC61AA-4F02-4DA9-BD34-21A4CDC1CA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD29E24-F64E-4572-ACB4-B3506AB19CFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2010" windowWidth="29040" windowHeight="17640" tabRatio="330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan BA" sheetId="11" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="Woche_anzeigen">'Zeitplan BA'!$M$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt einen Projektplan.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -106,9 +105,6 @@
 Fügen Sie ÜBER dieser Zeile neue Zeilen ein, um mit der Erstellung Ihres Projektplans fortzufahren.</t>
   </si>
   <si>
-    <t>Neue Zeilen ÜBER dieser einfügen</t>
-  </si>
-  <si>
     <t>START</t>
   </si>
   <si>
@@ -127,13 +123,7 @@
     <t>Schreibphase</t>
   </si>
   <si>
-    <t>Ausschreibung</t>
-  </si>
-  <si>
     <t>Vertrag</t>
-  </si>
-  <si>
-    <t>Besprechung Thema</t>
   </si>
   <si>
     <t>Literatursuche &amp; -analyse</t>
@@ -184,9 +174,6 @@
     <t>Deckbaltt, Kurzfassunng/Abstract, Einleitung</t>
   </si>
   <si>
-    <t>Grundlagen: Data Science Workflow, Big Data</t>
-  </si>
-  <si>
     <t>Evaluation</t>
   </si>
   <si>
@@ -229,7 +216,16 @@
     <t>Project End:</t>
   </si>
   <si>
-    <t>JavaScript recherchieren</t>
+    <t>Proposal/Ausschreibung</t>
+  </si>
+  <si>
+    <t>Aufgabenteile erstellen</t>
+  </si>
+  <si>
+    <t>Grundlagen: JavaScript, Asynchronous Programming, Software Quality</t>
+  </si>
+  <si>
+    <t>Besprechung Aufgaben</t>
   </si>
 </sst>
 </file>
@@ -741,7 +737,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -971,21 +967,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFF0000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFFF0000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFFF0000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0" tint="-0.34998626667073579"/>
       </left>
       <right/>
@@ -1088,6 +1069,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1160,7 +1169,7 @@
     <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1406,34 +1415,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="171" fontId="9" fillId="0" borderId="17" xfId="9" applyNumberFormat="1" applyBorder="1">
@@ -1452,7 +1458,7 @@
     <xf numFmtId="169" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1460,6 +1466,12 @@
     </xf>
     <xf numFmtId="169" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2014,9 +2026,9 @@
   </sheetPr>
   <dimension ref="A1:BR47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN14" sqref="AN14"/>
+      <selection pane="bottomLeft" activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2037,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="82" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" s="83"/>
       <c r="D1" s="84"/>
@@ -2051,7 +2063,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H2" s="35"/>
     </row>
@@ -2060,390 +2072,390 @@
         <v>2</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="70"/>
       <c r="D3" s="81" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="95">
+        <v>47</v>
+      </c>
+      <c r="E3" s="94">
         <v>44683</v>
       </c>
-      <c r="F3" s="96"/>
+      <c r="F3" s="95"/>
       <c r="H3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" s="101">
-        <v>-1</v>
-      </c>
-      <c r="N3" s="101"/>
+        <v>46</v>
+      </c>
+      <c r="M3" s="100">
+        <v>0</v>
+      </c>
+      <c r="N3" s="100"/>
     </row>
     <row r="4" spans="1:70" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="95">
+        <v>49</v>
+      </c>
+      <c r="E4" s="94">
         <f>Projektanfang+184</f>
         <v>44867</v>
       </c>
-      <c r="F4" s="96"/>
-      <c r="H4" s="98">
+      <c r="F4" s="95"/>
+      <c r="H4" s="97">
         <f>H5</f>
-        <v>44669</v>
-      </c>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="103"/>
-      <c r="O4" s="98">
+        <v>44676</v>
+      </c>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="97">
         <f>O5</f>
-        <v>44676</v>
-      </c>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="100"/>
-      <c r="V4" s="98">
+        <v>44683</v>
+      </c>
+      <c r="P4" s="98"/>
+      <c r="Q4" s="98"/>
+      <c r="R4" s="98"/>
+      <c r="S4" s="98"/>
+      <c r="T4" s="98"/>
+      <c r="U4" s="99"/>
+      <c r="V4" s="97">
         <f>V5</f>
-        <v>44683</v>
-      </c>
-      <c r="W4" s="99"/>
-      <c r="X4" s="99"/>
-      <c r="Y4" s="99"/>
-      <c r="Z4" s="99"/>
-      <c r="AA4" s="99"/>
-      <c r="AB4" s="100"/>
-      <c r="AC4" s="98">
+        <v>44690</v>
+      </c>
+      <c r="W4" s="98"/>
+      <c r="X4" s="98"/>
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="98"/>
+      <c r="AA4" s="98"/>
+      <c r="AB4" s="99"/>
+      <c r="AC4" s="97">
         <f>AC5</f>
-        <v>44690</v>
-      </c>
-      <c r="AD4" s="99"/>
-      <c r="AE4" s="99"/>
-      <c r="AF4" s="99"/>
-      <c r="AG4" s="99"/>
-      <c r="AH4" s="99"/>
-      <c r="AI4" s="100"/>
-      <c r="AJ4" s="98">
+        <v>44697</v>
+      </c>
+      <c r="AD4" s="98"/>
+      <c r="AE4" s="98"/>
+      <c r="AF4" s="98"/>
+      <c r="AG4" s="98"/>
+      <c r="AH4" s="98"/>
+      <c r="AI4" s="99"/>
+      <c r="AJ4" s="97">
         <f>AJ5</f>
-        <v>44697</v>
-      </c>
-      <c r="AK4" s="99"/>
-      <c r="AL4" s="99"/>
-      <c r="AM4" s="99"/>
-      <c r="AN4" s="99"/>
-      <c r="AO4" s="99"/>
-      <c r="AP4" s="100"/>
-      <c r="AQ4" s="98">
+        <v>44704</v>
+      </c>
+      <c r="AK4" s="98"/>
+      <c r="AL4" s="98"/>
+      <c r="AM4" s="98"/>
+      <c r="AN4" s="98"/>
+      <c r="AO4" s="98"/>
+      <c r="AP4" s="99"/>
+      <c r="AQ4" s="97">
         <f>AQ5</f>
-        <v>44704</v>
-      </c>
-      <c r="AR4" s="99"/>
-      <c r="AS4" s="99"/>
-      <c r="AT4" s="99"/>
-      <c r="AU4" s="99"/>
-      <c r="AV4" s="99"/>
-      <c r="AW4" s="100"/>
-      <c r="AX4" s="98">
+        <v>44711</v>
+      </c>
+      <c r="AR4" s="98"/>
+      <c r="AS4" s="98"/>
+      <c r="AT4" s="98"/>
+      <c r="AU4" s="98"/>
+      <c r="AV4" s="98"/>
+      <c r="AW4" s="99"/>
+      <c r="AX4" s="97">
         <f>AX5</f>
-        <v>44711</v>
-      </c>
-      <c r="AY4" s="99"/>
-      <c r="AZ4" s="99"/>
-      <c r="BA4" s="99"/>
-      <c r="BB4" s="99"/>
-      <c r="BC4" s="99"/>
-      <c r="BD4" s="100"/>
-      <c r="BE4" s="98">
+        <v>44718</v>
+      </c>
+      <c r="AY4" s="98"/>
+      <c r="AZ4" s="98"/>
+      <c r="BA4" s="98"/>
+      <c r="BB4" s="98"/>
+      <c r="BC4" s="98"/>
+      <c r="BD4" s="99"/>
+      <c r="BE4" s="97">
         <f>BE5</f>
-        <v>44718</v>
-      </c>
-      <c r="BF4" s="99"/>
-      <c r="BG4" s="99"/>
-      <c r="BH4" s="99"/>
-      <c r="BI4" s="99"/>
-      <c r="BJ4" s="99"/>
-      <c r="BK4" s="100"/>
-      <c r="BL4" s="98">
+        <v>44725</v>
+      </c>
+      <c r="BF4" s="98"/>
+      <c r="BG4" s="98"/>
+      <c r="BH4" s="98"/>
+      <c r="BI4" s="98"/>
+      <c r="BJ4" s="98"/>
+      <c r="BK4" s="99"/>
+      <c r="BL4" s="97">
         <f>BL5</f>
-        <v>44725</v>
-      </c>
-      <c r="BM4" s="99"/>
-      <c r="BN4" s="99"/>
-      <c r="BO4" s="99"/>
-      <c r="BP4" s="99"/>
-      <c r="BQ4" s="99"/>
-      <c r="BR4" s="100"/>
+        <v>44732</v>
+      </c>
+      <c r="BM4" s="98"/>
+      <c r="BN4" s="98"/>
+      <c r="BO4" s="98"/>
+      <c r="BP4" s="98"/>
+      <c r="BQ4" s="98"/>
+      <c r="BR4" s="99"/>
     </row>
     <row r="5" spans="1:70" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
       <c r="H5" s="55">
         <f>Projektanfang-WEEKDAY(Projektanfang,1)+2+7*(Woche_anzeigen-1)</f>
-        <v>44669</v>
+        <v>44676</v>
       </c>
       <c r="I5" s="56">
         <f>H5+1</f>
-        <v>44670</v>
+        <v>44677</v>
       </c>
       <c r="J5" s="56">
         <f t="shared" ref="J5:AW5" si="0">I5+1</f>
-        <v>44671</v>
+        <v>44678</v>
       </c>
       <c r="K5" s="56">
         <f t="shared" si="0"/>
-        <v>44672</v>
+        <v>44679</v>
       </c>
       <c r="L5" s="56">
         <f t="shared" si="0"/>
-        <v>44673</v>
+        <v>44680</v>
       </c>
       <c r="M5" s="56">
         <f t="shared" si="0"/>
-        <v>44674</v>
+        <v>44681</v>
       </c>
       <c r="N5" s="57">
         <f t="shared" si="0"/>
-        <v>44675</v>
+        <v>44682</v>
       </c>
       <c r="O5" s="55">
         <f>N5+1</f>
-        <v>44676</v>
+        <v>44683</v>
       </c>
       <c r="P5" s="56">
         <f>O5+1</f>
-        <v>44677</v>
+        <v>44684</v>
       </c>
       <c r="Q5" s="56">
         <f t="shared" si="0"/>
-        <v>44678</v>
+        <v>44685</v>
       </c>
       <c r="R5" s="56">
         <f t="shared" si="0"/>
-        <v>44679</v>
+        <v>44686</v>
       </c>
       <c r="S5" s="56">
         <f t="shared" si="0"/>
-        <v>44680</v>
+        <v>44687</v>
       </c>
       <c r="T5" s="56">
         <f t="shared" si="0"/>
-        <v>44681</v>
+        <v>44688</v>
       </c>
       <c r="U5" s="57">
         <f t="shared" si="0"/>
-        <v>44682</v>
+        <v>44689</v>
       </c>
       <c r="V5" s="55">
         <f>U5+1</f>
-        <v>44683</v>
+        <v>44690</v>
       </c>
       <c r="W5" s="56">
         <f>V5+1</f>
-        <v>44684</v>
+        <v>44691</v>
       </c>
       <c r="X5" s="56">
         <f t="shared" si="0"/>
-        <v>44685</v>
+        <v>44692</v>
       </c>
       <c r="Y5" s="56">
         <f t="shared" si="0"/>
-        <v>44686</v>
+        <v>44693</v>
       </c>
       <c r="Z5" s="56">
         <f t="shared" si="0"/>
-        <v>44687</v>
+        <v>44694</v>
       </c>
       <c r="AA5" s="56">
         <f t="shared" si="0"/>
-        <v>44688</v>
+        <v>44695</v>
       </c>
       <c r="AB5" s="57">
         <f t="shared" si="0"/>
-        <v>44689</v>
+        <v>44696</v>
       </c>
       <c r="AC5" s="55">
         <f>AB5+1</f>
-        <v>44690</v>
+        <v>44697</v>
       </c>
       <c r="AD5" s="56">
         <f>AC5+1</f>
-        <v>44691</v>
+        <v>44698</v>
       </c>
       <c r="AE5" s="56">
         <f t="shared" si="0"/>
-        <v>44692</v>
+        <v>44699</v>
       </c>
       <c r="AF5" s="56">
         <f t="shared" si="0"/>
-        <v>44693</v>
+        <v>44700</v>
       </c>
       <c r="AG5" s="56">
         <f t="shared" si="0"/>
-        <v>44694</v>
+        <v>44701</v>
       </c>
       <c r="AH5" s="56">
         <f t="shared" si="0"/>
-        <v>44695</v>
+        <v>44702</v>
       </c>
       <c r="AI5" s="57">
         <f t="shared" si="0"/>
-        <v>44696</v>
+        <v>44703</v>
       </c>
       <c r="AJ5" s="55">
         <f>AI5+1</f>
-        <v>44697</v>
+        <v>44704</v>
       </c>
       <c r="AK5" s="56">
         <f>AJ5+1</f>
-        <v>44698</v>
+        <v>44705</v>
       </c>
       <c r="AL5" s="56">
         <f t="shared" si="0"/>
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="AM5" s="56">
         <f t="shared" si="0"/>
-        <v>44700</v>
+        <v>44707</v>
       </c>
       <c r="AN5" s="56">
         <f t="shared" si="0"/>
-        <v>44701</v>
+        <v>44708</v>
       </c>
       <c r="AO5" s="56">
         <f t="shared" si="0"/>
-        <v>44702</v>
+        <v>44709</v>
       </c>
       <c r="AP5" s="57">
         <f t="shared" si="0"/>
-        <v>44703</v>
+        <v>44710</v>
       </c>
       <c r="AQ5" s="55">
         <f>AP5+1</f>
-        <v>44704</v>
+        <v>44711</v>
       </c>
       <c r="AR5" s="56">
         <f>AQ5+1</f>
-        <v>44705</v>
+        <v>44712</v>
       </c>
       <c r="AS5" s="56">
         <f t="shared" si="0"/>
-        <v>44706</v>
+        <v>44713</v>
       </c>
       <c r="AT5" s="56">
         <f t="shared" si="0"/>
-        <v>44707</v>
+        <v>44714</v>
       </c>
       <c r="AU5" s="56">
         <f t="shared" si="0"/>
-        <v>44708</v>
+        <v>44715</v>
       </c>
       <c r="AV5" s="56">
         <f t="shared" si="0"/>
-        <v>44709</v>
+        <v>44716</v>
       </c>
       <c r="AW5" s="57">
         <f t="shared" si="0"/>
-        <v>44710</v>
+        <v>44717</v>
       </c>
       <c r="AX5" s="55">
         <f>AW5+1</f>
-        <v>44711</v>
+        <v>44718</v>
       </c>
       <c r="AY5" s="56">
         <f>AX5+1</f>
-        <v>44712</v>
+        <v>44719</v>
       </c>
       <c r="AZ5" s="56">
         <f t="shared" ref="AZ5:BD5" si="1">AY5+1</f>
-        <v>44713</v>
+        <v>44720</v>
       </c>
       <c r="BA5" s="56">
         <f t="shared" si="1"/>
-        <v>44714</v>
+        <v>44721</v>
       </c>
       <c r="BB5" s="56">
         <f t="shared" si="1"/>
-        <v>44715</v>
+        <v>44722</v>
       </c>
       <c r="BC5" s="56">
         <f t="shared" si="1"/>
-        <v>44716</v>
+        <v>44723</v>
       </c>
       <c r="BD5" s="57">
         <f t="shared" si="1"/>
-        <v>44717</v>
+        <v>44724</v>
       </c>
       <c r="BE5" s="55">
         <f>BD5+1</f>
-        <v>44718</v>
+        <v>44725</v>
       </c>
       <c r="BF5" s="56">
         <f>BE5+1</f>
-        <v>44719</v>
+        <v>44726</v>
       </c>
       <c r="BG5" s="56">
         <f t="shared" ref="BG5:BK5" si="2">BF5+1</f>
-        <v>44720</v>
+        <v>44727</v>
       </c>
       <c r="BH5" s="56">
         <f t="shared" si="2"/>
-        <v>44721</v>
+        <v>44728</v>
       </c>
       <c r="BI5" s="56">
         <f t="shared" si="2"/>
-        <v>44722</v>
+        <v>44729</v>
       </c>
       <c r="BJ5" s="56">
         <f t="shared" si="2"/>
-        <v>44723</v>
+        <v>44730</v>
       </c>
       <c r="BK5" s="57">
         <f t="shared" si="2"/>
-        <v>44724</v>
+        <v>44731</v>
       </c>
       <c r="BL5" s="55">
         <f>BK5+1</f>
-        <v>44725</v>
+        <v>44732</v>
       </c>
       <c r="BM5" s="56">
         <f>BL5+1</f>
-        <v>44726</v>
+        <v>44733</v>
       </c>
       <c r="BN5" s="56">
         <f t="shared" ref="BN5" si="3">BM5+1</f>
-        <v>44727</v>
+        <v>44734</v>
       </c>
       <c r="BO5" s="56">
-        <f t="shared" ref="BO5" si="4">BN5+1</f>
-        <v>44728</v>
+        <f>BN5+1</f>
+        <v>44735</v>
       </c>
       <c r="BP5" s="56">
-        <f t="shared" ref="BP5" si="5">BO5+1</f>
-        <v>44729</v>
+        <f t="shared" ref="BP5" si="4">BO5+1</f>
+        <v>44736</v>
       </c>
       <c r="BQ5" s="56">
-        <f t="shared" ref="BQ5" si="6">BP5+1</f>
-        <v>44730</v>
+        <f t="shared" ref="BQ5" si="5">BP5+1</f>
+        <v>44737</v>
       </c>
       <c r="BR5" s="57">
-        <f t="shared" ref="BR5" si="7">BQ5+1</f>
-        <v>44731</v>
+        <f t="shared" ref="BR5" si="6">BQ5+1</f>
+        <v>44738</v>
       </c>
     </row>
     <row r="6" spans="1:70" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2451,271 +2463,271 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H6" s="7" t="str">
-        <f t="shared" ref="H6:AM6" si="8">LEFT(TEXT(H5,"TTT"),1)</f>
+        <f t="shared" ref="H6:AM6" si="7">LEFT(TEXT(H5,"TTT"),1)</f>
         <v>M</v>
       </c>
       <c r="I6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>D</v>
+      </c>
+      <c r="J6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>M</v>
+      </c>
+      <c r="K6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>D</v>
+      </c>
+      <c r="L6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>F</v>
+      </c>
+      <c r="M6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="N6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="O6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>M</v>
+      </c>
+      <c r="P6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>D</v>
+      </c>
+      <c r="Q6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>M</v>
+      </c>
+      <c r="R6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>D</v>
+      </c>
+      <c r="S6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>F</v>
+      </c>
+      <c r="T6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="U6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="V6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>M</v>
+      </c>
+      <c r="W6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>D</v>
+      </c>
+      <c r="X6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>M</v>
+      </c>
+      <c r="Y6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>D</v>
+      </c>
+      <c r="Z6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>F</v>
+      </c>
+      <c r="AA6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="AB6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="AC6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>M</v>
+      </c>
+      <c r="AD6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>D</v>
+      </c>
+      <c r="AE6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>M</v>
+      </c>
+      <c r="AF6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>D</v>
+      </c>
+      <c r="AG6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>F</v>
+      </c>
+      <c r="AH6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="AI6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>S</v>
+      </c>
+      <c r="AJ6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>M</v>
+      </c>
+      <c r="AK6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>D</v>
+      </c>
+      <c r="AL6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>M</v>
+      </c>
+      <c r="AM6" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>D</v>
+      </c>
+      <c r="AN6" s="7" t="str">
+        <f t="shared" ref="AN6:BK6" si="8">LEFT(TEXT(AN5,"TTT"),1)</f>
+        <v>F</v>
+      </c>
+      <c r="AO6" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="AP6" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>S</v>
+      </c>
+      <c r="AQ6" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>M</v>
+      </c>
+      <c r="AR6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>D</v>
       </c>
-      <c r="J6" s="7" t="str">
+      <c r="AS6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>M</v>
       </c>
-      <c r="K6" s="7" t="str">
+      <c r="AT6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>D</v>
       </c>
-      <c r="L6" s="7" t="str">
+      <c r="AU6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>F</v>
       </c>
-      <c r="M6" s="7" t="str">
+      <c r="AV6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>S</v>
       </c>
-      <c r="N6" s="7" t="str">
+      <c r="AW6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>S</v>
       </c>
-      <c r="O6" s="7" t="str">
+      <c r="AX6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>M</v>
       </c>
-      <c r="P6" s="7" t="str">
+      <c r="AY6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>D</v>
       </c>
-      <c r="Q6" s="7" t="str">
+      <c r="AZ6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>M</v>
       </c>
-      <c r="R6" s="7" t="str">
+      <c r="BA6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>D</v>
       </c>
-      <c r="S6" s="7" t="str">
+      <c r="BB6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>F</v>
       </c>
-      <c r="T6" s="7" t="str">
+      <c r="BC6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>S</v>
       </c>
-      <c r="U6" s="7" t="str">
+      <c r="BD6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>S</v>
       </c>
-      <c r="V6" s="7" t="str">
+      <c r="BE6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>M</v>
       </c>
-      <c r="W6" s="7" t="str">
+      <c r="BF6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>D</v>
       </c>
-      <c r="X6" s="7" t="str">
+      <c r="BG6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>M</v>
       </c>
-      <c r="Y6" s="7" t="str">
+      <c r="BH6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>D</v>
       </c>
-      <c r="Z6" s="7" t="str">
+      <c r="BI6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>F</v>
       </c>
-      <c r="AA6" s="7" t="str">
+      <c r="BJ6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>S</v>
       </c>
-      <c r="AB6" s="7" t="str">
+      <c r="BK6" s="7" t="str">
         <f t="shared" si="8"/>
         <v>S</v>
       </c>
-      <c r="AC6" s="7" t="str">
-        <f t="shared" si="8"/>
+      <c r="BL6" s="7" t="str">
+        <f t="shared" ref="BL6:BR6" si="9">LEFT(TEXT(BL5,"TTT"),1)</f>
         <v>M</v>
       </c>
-      <c r="AD6" s="7" t="str">
-        <f t="shared" si="8"/>
+      <c r="BM6" s="7" t="str">
+        <f t="shared" si="9"/>
         <v>D</v>
       </c>
-      <c r="AE6" s="7" t="str">
-        <f t="shared" si="8"/>
+      <c r="BN6" s="85" t="str">
+        <f t="shared" si="9"/>
         <v>M</v>
       </c>
-      <c r="AF6" s="7" t="str">
-        <f t="shared" si="8"/>
+      <c r="BO6" s="104" t="str">
+        <f t="shared" si="9"/>
         <v>D</v>
       </c>
-      <c r="AG6" s="7" t="str">
-        <f t="shared" si="8"/>
+      <c r="BP6" s="86" t="str">
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
-      <c r="AH6" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="AI6" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>S</v>
-      </c>
-      <c r="AJ6" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>M</v>
-      </c>
-      <c r="AK6" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>D</v>
-      </c>
-      <c r="AL6" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>M</v>
-      </c>
-      <c r="AM6" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>D</v>
-      </c>
-      <c r="AN6" s="7" t="str">
-        <f t="shared" ref="AN6:BK6" si="9">LEFT(TEXT(AN5,"TTT"),1)</f>
-        <v>F</v>
-      </c>
-      <c r="AO6" s="7" t="str">
+      <c r="BQ6" s="7" t="str">
         <f t="shared" si="9"/>
         <v>S</v>
       </c>
-      <c r="AP6" s="7" t="str">
+      <c r="BR6" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="AQ6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>M</v>
-      </c>
-      <c r="AR6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>D</v>
-      </c>
-      <c r="AS6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>M</v>
-      </c>
-      <c r="AT6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>D</v>
-      </c>
-      <c r="AU6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>F</v>
-      </c>
-      <c r="AV6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="AW6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="AX6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>M</v>
-      </c>
-      <c r="AY6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>D</v>
-      </c>
-      <c r="AZ6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>M</v>
-      </c>
-      <c r="BA6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>D</v>
-      </c>
-      <c r="BB6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>F</v>
-      </c>
-      <c r="BC6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="BD6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="BE6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>M</v>
-      </c>
-      <c r="BF6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>D</v>
-      </c>
-      <c r="BG6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>M</v>
-      </c>
-      <c r="BH6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>D</v>
-      </c>
-      <c r="BI6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>F</v>
-      </c>
-      <c r="BJ6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="BK6" s="7" t="str">
-        <f t="shared" si="9"/>
-        <v>S</v>
-      </c>
-      <c r="BL6" s="7" t="str">
-        <f t="shared" ref="BL6:BR6" si="10">LEFT(TEXT(BL5,"TTT"),1)</f>
-        <v>M</v>
-      </c>
-      <c r="BM6" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>D</v>
-      </c>
-      <c r="BN6" s="85" t="str">
-        <f t="shared" si="10"/>
-        <v>M</v>
-      </c>
-      <c r="BO6" s="87" t="str">
-        <f t="shared" si="10"/>
-        <v>D</v>
-      </c>
-      <c r="BP6" s="86" t="str">
-        <f t="shared" si="10"/>
-        <v>F</v>
-      </c>
-      <c r="BQ6" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>S</v>
-      </c>
-      <c r="BR6" s="7" t="str">
-        <f t="shared" si="10"/>
         <v>S</v>
       </c>
     </row>
@@ -2724,14 +2736,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="38"/>
       <c r="D7" s="16"/>
       <c r="E7" s="61"/>
       <c r="F7" s="62"/>
       <c r="G7" s="11" t="str">
-        <f t="shared" ref="G7:G12" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="G7:G12" si="10">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="H7" s="28"/>
@@ -2792,15 +2804,15 @@
       <c r="BK7" s="28"/>
       <c r="BL7" s="28"/>
       <c r="BM7" s="28"/>
-      <c r="BN7" s="90"/>
-      <c r="BO7" s="88"/>
+      <c r="BN7" s="89"/>
+      <c r="BO7" s="103"/>
       <c r="BP7" s="28"/>
       <c r="BQ7" s="28"/>
       <c r="BR7" s="28"/>
     </row>
     <row r="8" spans="1:70" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="46" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8" s="39"/>
       <c r="D8" s="17">
@@ -2814,7 +2826,7 @@
         <v>44661</v>
       </c>
       <c r="G8" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H8" s="28"/>
@@ -2875,15 +2887,15 @@
       <c r="BK8" s="28"/>
       <c r="BL8" s="28"/>
       <c r="BM8" s="28"/>
-      <c r="BN8" s="90"/>
-      <c r="BO8" s="88"/>
+      <c r="BN8" s="89"/>
+      <c r="BO8" s="87"/>
       <c r="BP8" s="28"/>
       <c r="BQ8" s="28"/>
       <c r="BR8" s="28"/>
     </row>
     <row r="9" spans="1:70" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="17">
@@ -2897,7 +2909,7 @@
         <v>44661</v>
       </c>
       <c r="G9" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="H9" s="28"/>
@@ -2958,15 +2970,15 @@
       <c r="BK9" s="28"/>
       <c r="BL9" s="28"/>
       <c r="BM9" s="28"/>
-      <c r="BN9" s="90"/>
-      <c r="BO9" s="88"/>
+      <c r="BN9" s="89"/>
+      <c r="BO9" s="87"/>
       <c r="BP9" s="28"/>
       <c r="BQ9" s="28"/>
       <c r="BR9" s="28"/>
     </row>
     <row r="10" spans="1:70" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="46" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="17">
@@ -2976,12 +2988,12 @@
         <v>44661</v>
       </c>
       <c r="F10" s="63">
-        <f>E10+0</f>
-        <v>44661</v>
+        <f>E10+30</f>
+        <v>44691</v>
       </c>
       <c r="G10" s="11">
-        <f t="shared" si="11"/>
-        <v>1</v>
+        <f t="shared" si="10"/>
+        <v>31</v>
       </c>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
@@ -3041,31 +3053,31 @@
       <c r="BK10" s="28"/>
       <c r="BL10" s="28"/>
       <c r="BM10" s="28"/>
-      <c r="BN10" s="90"/>
-      <c r="BO10" s="88"/>
+      <c r="BN10" s="89"/>
+      <c r="BO10" s="87"/>
       <c r="BP10" s="28"/>
       <c r="BQ10" s="28"/>
       <c r="BR10" s="28"/>
     </row>
     <row r="11" spans="1:70" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="46" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="17">
         <v>0.3</v>
       </c>
       <c r="E11" s="63">
-        <f>E10</f>
-        <v>44661</v>
+        <f>F10+1</f>
+        <v>44692</v>
       </c>
       <c r="F11" s="63">
-        <f>E11+30</f>
-        <v>44691</v>
+        <f>E11+10</f>
+        <v>44702</v>
       </c>
       <c r="G11" s="11">
-        <f t="shared" si="11"/>
-        <v>31</v>
+        <f t="shared" si="10"/>
+        <v>11</v>
       </c>
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
@@ -3125,19 +3137,19 @@
       <c r="BK11" s="28"/>
       <c r="BL11" s="28"/>
       <c r="BM11" s="28"/>
-      <c r="BN11" s="90"/>
-      <c r="BO11" s="88"/>
+      <c r="BN11" s="89"/>
+      <c r="BO11" s="87"/>
       <c r="BP11" s="28"/>
       <c r="BQ11" s="28"/>
       <c r="BR11" s="28"/>
     </row>
     <row r="12" spans="1:70" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="46" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="17">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E12" s="63">
         <v>44662</v>
@@ -3147,7 +3159,7 @@
         <v>44682</v>
       </c>
       <c r="G12" s="11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="H12" s="28"/>
@@ -3208,8 +3220,8 @@
       <c r="BK12" s="28"/>
       <c r="BL12" s="28"/>
       <c r="BM12" s="28"/>
-      <c r="BN12" s="90"/>
-      <c r="BO12" s="88"/>
+      <c r="BN12" s="89"/>
+      <c r="BO12" s="87"/>
       <c r="BP12" s="28"/>
       <c r="BQ12" s="28"/>
       <c r="BR12" s="28"/>
@@ -3219,14 +3231,14 @@
         <v>7</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="36"/>
       <c r="D13" s="13"/>
       <c r="E13" s="50"/>
       <c r="F13" s="51"/>
       <c r="G13" s="11" t="str">
-        <f t="shared" ref="G13:G44" si="12">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="G13:G44" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="H13" s="28"/>
@@ -3287,8 +3299,8 @@
       <c r="BK13" s="28"/>
       <c r="BL13" s="28"/>
       <c r="BM13" s="28"/>
-      <c r="BN13" s="90"/>
-      <c r="BO13" s="89"/>
+      <c r="BN13" s="89"/>
+      <c r="BO13" s="88"/>
       <c r="BP13" s="28"/>
       <c r="BQ13" s="28"/>
       <c r="BR13" s="28"/>
@@ -3298,22 +3310,22 @@
         <v>8</v>
       </c>
       <c r="B14" s="45" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="14">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E14" s="60">
         <v>44671</v>
       </c>
       <c r="F14" s="60">
-        <f>E14+3</f>
-        <v>44674</v>
+        <f>E14+9</f>
+        <v>44680</v>
       </c>
       <c r="G14" s="11">
-        <f t="shared" si="12"/>
-        <v>4</v>
+        <f t="shared" si="11"/>
+        <v>10</v>
       </c>
       <c r="H14" s="80"/>
       <c r="I14" s="80"/>
@@ -3373,8 +3385,8 @@
       <c r="BK14" s="28"/>
       <c r="BL14" s="28"/>
       <c r="BM14" s="28"/>
-      <c r="BN14" s="90"/>
-      <c r="BO14" s="89"/>
+      <c r="BN14" s="89"/>
+      <c r="BO14" s="88"/>
       <c r="BP14" s="28"/>
       <c r="BQ14" s="28"/>
       <c r="BR14" s="28"/>
@@ -3384,7 +3396,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C15" s="37"/>
       <c r="D15" s="14">
@@ -3392,15 +3404,15 @@
       </c>
       <c r="E15" s="60">
         <f>F14+2</f>
-        <v>44676</v>
+        <v>44682</v>
       </c>
       <c r="F15" s="60">
-        <f>E15+5</f>
-        <v>44681</v>
+        <f>E15+6</f>
+        <v>44688</v>
       </c>
       <c r="G15" s="11">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
@@ -3460,8 +3472,8 @@
       <c r="BK15" s="28"/>
       <c r="BL15" s="28"/>
       <c r="BM15" s="28"/>
-      <c r="BN15" s="90"/>
-      <c r="BO15" s="89"/>
+      <c r="BN15" s="89"/>
+      <c r="BO15" s="88"/>
       <c r="BP15" s="28"/>
       <c r="BQ15" s="28"/>
       <c r="BR15" s="28"/>
@@ -3469,22 +3481,22 @@
     <row r="16" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32"/>
       <c r="B16" s="45" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="C16" s="37"/>
       <c r="D16" s="14">
         <v>0</v>
       </c>
       <c r="E16" s="60">
-        <f>F15+2</f>
-        <v>44683</v>
+        <f>F15+1</f>
+        <v>44689</v>
       </c>
       <c r="F16" s="60">
         <f>E16+0</f>
-        <v>44683</v>
+        <v>44689</v>
       </c>
       <c r="G16" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="H16" s="28"/>
@@ -3545,8 +3557,8 @@
       <c r="BK16" s="28"/>
       <c r="BL16" s="28"/>
       <c r="BM16" s="28"/>
-      <c r="BN16" s="90"/>
-      <c r="BO16" s="89"/>
+      <c r="BN16" s="89"/>
+      <c r="BO16" s="88"/>
       <c r="BP16" s="28"/>
       <c r="BQ16" s="28"/>
       <c r="BR16" s="28"/>
@@ -3556,14 +3568,14 @@
         <v>10</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="40"/>
       <c r="D17" s="19"/>
       <c r="E17" s="64"/>
       <c r="F17" s="65"/>
       <c r="G17" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H17" s="28"/>
@@ -3624,8 +3636,8 @@
       <c r="BK17" s="28"/>
       <c r="BL17" s="28"/>
       <c r="BM17" s="28"/>
-      <c r="BN17" s="90"/>
-      <c r="BO17" s="89"/>
+      <c r="BN17" s="89"/>
+      <c r="BO17" s="88"/>
       <c r="BP17" s="28"/>
       <c r="BQ17" s="28"/>
       <c r="BR17" s="28"/>
@@ -3633,7 +3645,7 @@
     <row r="18" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32"/>
       <c r="B18" s="47" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="20">
@@ -3647,7 +3659,7 @@
         <v>44684</v>
       </c>
       <c r="G18" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="H18" s="28"/>
@@ -3708,8 +3720,8 @@
       <c r="BK18" s="28"/>
       <c r="BL18" s="28"/>
       <c r="BM18" s="28"/>
-      <c r="BN18" s="90"/>
-      <c r="BO18" s="89"/>
+      <c r="BN18" s="89"/>
+      <c r="BO18" s="88"/>
       <c r="BP18" s="28"/>
       <c r="BQ18" s="28"/>
       <c r="BR18" s="28"/>
@@ -3717,7 +3729,7 @@
     <row r="19" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32"/>
       <c r="B19" s="47" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="20">
@@ -3732,7 +3744,7 @@
         <v>44689</v>
       </c>
       <c r="G19" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="H19" s="28"/>
@@ -3793,8 +3805,8 @@
       <c r="BK19" s="28"/>
       <c r="BL19" s="28"/>
       <c r="BM19" s="28"/>
-      <c r="BN19" s="90"/>
-      <c r="BO19" s="89"/>
+      <c r="BN19" s="89"/>
+      <c r="BO19" s="88"/>
       <c r="BP19" s="28"/>
       <c r="BQ19" s="28"/>
       <c r="BR19" s="28"/>
@@ -3812,7 +3824,7 @@
         <v>44707</v>
       </c>
       <c r="G20" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="H20" s="28"/>
@@ -3873,8 +3885,8 @@
       <c r="BK20" s="28"/>
       <c r="BL20" s="28"/>
       <c r="BM20" s="28"/>
-      <c r="BN20" s="90"/>
-      <c r="BO20" s="89"/>
+      <c r="BN20" s="89"/>
+      <c r="BO20" s="88"/>
       <c r="BP20" s="28"/>
       <c r="BQ20" s="28"/>
       <c r="BR20" s="28"/>
@@ -3893,7 +3905,7 @@
         <v>44712</v>
       </c>
       <c r="G21" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="H21" s="28"/>
@@ -3954,8 +3966,8 @@
       <c r="BK21" s="28"/>
       <c r="BL21" s="28"/>
       <c r="BM21" s="28"/>
-      <c r="BN21" s="90"/>
-      <c r="BO21" s="89"/>
+      <c r="BN21" s="89"/>
+      <c r="BO21" s="88"/>
       <c r="BP21" s="28"/>
       <c r="BQ21" s="28"/>
       <c r="BR21" s="28"/>
@@ -3974,7 +3986,7 @@
         <v>44707</v>
       </c>
       <c r="G22" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="H22" s="28"/>
@@ -4035,8 +4047,8 @@
       <c r="BK22" s="28"/>
       <c r="BL22" s="28"/>
       <c r="BM22" s="28"/>
-      <c r="BN22" s="90"/>
-      <c r="BO22" s="89"/>
+      <c r="BN22" s="89"/>
+      <c r="BO22" s="88"/>
       <c r="BP22" s="28"/>
       <c r="BQ22" s="28"/>
       <c r="BR22" s="28"/>
@@ -4046,14 +4058,14 @@
         <v>10</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23" s="76"/>
       <c r="D23" s="77"/>
       <c r="E23" s="78"/>
       <c r="F23" s="79"/>
       <c r="G23" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H23" s="28"/>
@@ -4114,8 +4126,8 @@
       <c r="BK23" s="28"/>
       <c r="BL23" s="28"/>
       <c r="BM23" s="28"/>
-      <c r="BN23" s="90"/>
-      <c r="BO23" s="89"/>
+      <c r="BN23" s="89"/>
+      <c r="BO23" s="88"/>
       <c r="BP23" s="28"/>
       <c r="BQ23" s="28"/>
       <c r="BR23" s="28"/>
@@ -4123,14 +4135,14 @@
     <row r="24" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="32"/>
       <c r="B24" s="75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="76"/>
       <c r="D24" s="77"/>
       <c r="E24" s="78"/>
       <c r="F24" s="79"/>
       <c r="G24" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H24" s="28"/>
@@ -4191,9 +4203,9 @@
       <c r="BK24" s="28"/>
       <c r="BL24" s="28"/>
       <c r="BM24" s="28"/>
-      <c r="BN24" s="90"/>
-      <c r="BO24" s="91"/>
-      <c r="BP24" s="89"/>
+      <c r="BN24" s="89"/>
+      <c r="BO24" s="90"/>
+      <c r="BP24" s="88"/>
       <c r="BQ24" s="28"/>
       <c r="BR24" s="28"/>
     </row>
@@ -4271,9 +4283,9 @@
       <c r="BK25" s="28"/>
       <c r="BL25" s="28"/>
       <c r="BM25" s="28"/>
-      <c r="BN25" s="90"/>
-      <c r="BO25" s="91"/>
-      <c r="BP25" s="89"/>
+      <c r="BN25" s="89"/>
+      <c r="BO25" s="90"/>
+      <c r="BP25" s="88"/>
       <c r="BQ25" s="28"/>
       <c r="BR25" s="28"/>
     </row>
@@ -4291,7 +4303,7 @@
         <v>44723</v>
       </c>
       <c r="G26" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="H26" s="28"/>
@@ -4352,9 +4364,9 @@
       <c r="BK26" s="28"/>
       <c r="BL26" s="28"/>
       <c r="BM26" s="28"/>
-      <c r="BN26" s="90"/>
-      <c r="BO26" s="91"/>
-      <c r="BP26" s="89"/>
+      <c r="BN26" s="89"/>
+      <c r="BO26" s="90"/>
+      <c r="BP26" s="88"/>
       <c r="BQ26" s="28"/>
       <c r="BR26" s="28"/>
     </row>
@@ -4372,7 +4384,7 @@
         <v>44733</v>
       </c>
       <c r="G27" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="H27" s="28"/>
@@ -4433,9 +4445,9 @@
       <c r="BK27" s="28"/>
       <c r="BL27" s="28"/>
       <c r="BM27" s="28"/>
-      <c r="BN27" s="90"/>
-      <c r="BO27" s="91"/>
-      <c r="BP27" s="89"/>
+      <c r="BN27" s="89"/>
+      <c r="BO27" s="90"/>
+      <c r="BP27" s="88"/>
       <c r="BQ27" s="28"/>
       <c r="BR27" s="28"/>
     </row>
@@ -4444,14 +4456,14 @@
         <v>11</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="36"/>
       <c r="D28" s="13"/>
       <c r="E28" s="50"/>
       <c r="F28" s="51"/>
       <c r="G28" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H28" s="28"/>
@@ -4512,16 +4524,16 @@
       <c r="BK28" s="28"/>
       <c r="BL28" s="28"/>
       <c r="BM28" s="28"/>
-      <c r="BN28" s="90"/>
-      <c r="BO28" s="91"/>
-      <c r="BP28" s="89"/>
+      <c r="BN28" s="89"/>
+      <c r="BO28" s="90"/>
+      <c r="BP28" s="88"/>
       <c r="BQ28" s="28"/>
       <c r="BR28" s="28"/>
     </row>
     <row r="29" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="32"/>
       <c r="B29" s="45" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C29" s="37"/>
       <c r="D29" s="14">
@@ -4536,7 +4548,7 @@
         <v>44735</v>
       </c>
       <c r="G29" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="H29" s="28"/>
@@ -4597,16 +4609,16 @@
       <c r="BK29" s="28"/>
       <c r="BL29" s="28"/>
       <c r="BM29" s="28"/>
-      <c r="BN29" s="90"/>
-      <c r="BO29" s="91"/>
-      <c r="BP29" s="89"/>
+      <c r="BN29" s="89"/>
+      <c r="BO29" s="90"/>
+      <c r="BP29" s="88"/>
       <c r="BQ29" s="28"/>
       <c r="BR29" s="28"/>
     </row>
     <row r="30" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="32"/>
       <c r="B30" s="45" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C30" s="37"/>
       <c r="D30" s="14">
@@ -4621,7 +4633,7 @@
         <v>44738</v>
       </c>
       <c r="G30" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="H30" s="28"/>
@@ -4682,16 +4694,16 @@
       <c r="BK30" s="28"/>
       <c r="BL30" s="28"/>
       <c r="BM30" s="28"/>
-      <c r="BN30" s="90"/>
-      <c r="BO30" s="91"/>
-      <c r="BP30" s="89"/>
+      <c r="BN30" s="89"/>
+      <c r="BO30" s="90"/>
+      <c r="BP30" s="88"/>
       <c r="BQ30" s="28"/>
       <c r="BR30" s="28"/>
     </row>
     <row r="31" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="32"/>
       <c r="B31" s="45" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C31" s="37"/>
       <c r="D31" s="14">
@@ -4706,7 +4718,7 @@
         <v>44757</v>
       </c>
       <c r="G31" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="H31" s="28"/>
@@ -4767,16 +4779,16 @@
       <c r="BK31" s="28"/>
       <c r="BL31" s="28"/>
       <c r="BM31" s="28"/>
-      <c r="BN31" s="90"/>
-      <c r="BO31" s="91"/>
-      <c r="BP31" s="89"/>
+      <c r="BN31" s="89"/>
+      <c r="BO31" s="90"/>
+      <c r="BP31" s="88"/>
       <c r="BQ31" s="28"/>
       <c r="BR31" s="28"/>
     </row>
     <row r="32" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="32"/>
       <c r="B32" s="45" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C32" s="37"/>
       <c r="D32" s="14">
@@ -4791,7 +4803,7 @@
         <v>44762</v>
       </c>
       <c r="G32" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="H32" s="28"/>
@@ -4852,16 +4864,16 @@
       <c r="BK32" s="28"/>
       <c r="BL32" s="28"/>
       <c r="BM32" s="28"/>
-      <c r="BN32" s="90"/>
-      <c r="BO32" s="91"/>
-      <c r="BP32" s="89"/>
+      <c r="BN32" s="89"/>
+      <c r="BO32" s="90"/>
+      <c r="BP32" s="88"/>
       <c r="BQ32" s="28"/>
       <c r="BR32" s="28"/>
     </row>
     <row r="33" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="32"/>
       <c r="B33" s="45" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C33" s="37"/>
       <c r="D33" s="14">
@@ -4876,7 +4888,7 @@
         <v>44763</v>
       </c>
       <c r="G33" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="H33" s="28"/>
@@ -4937,16 +4949,16 @@
       <c r="BK33" s="28"/>
       <c r="BL33" s="28"/>
       <c r="BM33" s="28"/>
-      <c r="BN33" s="90"/>
-      <c r="BO33" s="91"/>
-      <c r="BP33" s="89"/>
+      <c r="BN33" s="89"/>
+      <c r="BO33" s="90"/>
+      <c r="BP33" s="88"/>
       <c r="BQ33" s="28"/>
       <c r="BR33" s="28"/>
     </row>
     <row r="34" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="32"/>
       <c r="B34" s="21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C34" s="42"/>
       <c r="D34" s="22"/>
@@ -5011,16 +5023,16 @@
       <c r="BK34" s="28"/>
       <c r="BL34" s="28"/>
       <c r="BM34" s="28"/>
-      <c r="BN34" s="90"/>
-      <c r="BO34" s="91"/>
-      <c r="BP34" s="89"/>
+      <c r="BN34" s="89"/>
+      <c r="BO34" s="90"/>
+      <c r="BP34" s="88"/>
       <c r="BQ34" s="28"/>
       <c r="BR34" s="28"/>
     </row>
     <row r="35" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="32"/>
       <c r="B35" s="48" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C35" s="43"/>
       <c r="D35" s="23">
@@ -5035,7 +5047,7 @@
         <v>44763</v>
       </c>
       <c r="G35" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="H35" s="28"/>
@@ -5096,16 +5108,16 @@
       <c r="BK35" s="28"/>
       <c r="BL35" s="28"/>
       <c r="BM35" s="28"/>
-      <c r="BN35" s="90"/>
-      <c r="BO35" s="91"/>
-      <c r="BP35" s="89"/>
+      <c r="BN35" s="89"/>
+      <c r="BO35" s="90"/>
+      <c r="BP35" s="88"/>
       <c r="BQ35" s="28"/>
       <c r="BR35" s="28"/>
     </row>
     <row r="36" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="32"/>
       <c r="B36" s="48" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C36" s="43"/>
       <c r="D36" s="23">
@@ -5120,7 +5132,7 @@
         <v>44765</v>
       </c>
       <c r="G36" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="H36" s="28"/>
@@ -5181,16 +5193,16 @@
       <c r="BK36" s="28"/>
       <c r="BL36" s="28"/>
       <c r="BM36" s="28"/>
-      <c r="BN36" s="90"/>
-      <c r="BO36" s="91"/>
-      <c r="BP36" s="89"/>
+      <c r="BN36" s="89"/>
+      <c r="BO36" s="90"/>
+      <c r="BP36" s="88"/>
       <c r="BQ36" s="28"/>
       <c r="BR36" s="28"/>
     </row>
     <row r="37" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="32"/>
       <c r="B37" s="48" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C37" s="43"/>
       <c r="D37" s="23">
@@ -5205,7 +5217,7 @@
         <v>44766</v>
       </c>
       <c r="G37" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="H37" s="28"/>
@@ -5266,16 +5278,16 @@
       <c r="BK37" s="28"/>
       <c r="BL37" s="28"/>
       <c r="BM37" s="28"/>
-      <c r="BN37" s="90"/>
-      <c r="BO37" s="91"/>
-      <c r="BP37" s="89"/>
+      <c r="BN37" s="89"/>
+      <c r="BO37" s="90"/>
+      <c r="BP37" s="88"/>
       <c r="BQ37" s="28"/>
       <c r="BR37" s="28"/>
     </row>
     <row r="38" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="32"/>
       <c r="B38" s="48" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C38" s="43"/>
       <c r="D38" s="23">
@@ -5351,16 +5363,16 @@
       <c r="BK38" s="28"/>
       <c r="BL38" s="28"/>
       <c r="BM38" s="28"/>
-      <c r="BN38" s="90"/>
-      <c r="BO38" s="91"/>
-      <c r="BP38" s="89"/>
+      <c r="BN38" s="89"/>
+      <c r="BO38" s="90"/>
+      <c r="BP38" s="88"/>
       <c r="BQ38" s="28"/>
       <c r="BR38" s="28"/>
     </row>
     <row r="39" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="32"/>
       <c r="B39" s="18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C39" s="40"/>
       <c r="D39" s="19"/>
@@ -5425,16 +5437,16 @@
       <c r="BK39" s="28"/>
       <c r="BL39" s="28"/>
       <c r="BM39" s="28"/>
-      <c r="BN39" s="90"/>
-      <c r="BO39" s="91"/>
-      <c r="BP39" s="89"/>
+      <c r="BN39" s="89"/>
+      <c r="BO39" s="90"/>
+      <c r="BP39" s="88"/>
       <c r="BQ39" s="28"/>
       <c r="BR39" s="28"/>
     </row>
     <row r="40" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="32"/>
       <c r="B40" s="47" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C40" s="41"/>
       <c r="D40" s="20">
@@ -5509,19 +5521,21 @@
       <c r="BK40" s="28"/>
       <c r="BL40" s="28"/>
       <c r="BM40" s="28"/>
-      <c r="BN40" s="90"/>
-      <c r="BO40" s="91"/>
-      <c r="BP40" s="89"/>
+      <c r="BN40" s="89"/>
+      <c r="BO40" s="90"/>
+      <c r="BP40" s="88"/>
       <c r="BQ40" s="28"/>
       <c r="BR40" s="28"/>
     </row>
     <row r="41" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="32"/>
       <c r="B41" s="47" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C41" s="41"/>
-      <c r="D41" s="20"/>
+      <c r="D41" s="20">
+        <v>0</v>
+      </c>
       <c r="E41" s="66">
         <v>44890</v>
       </c>
@@ -5591,16 +5605,16 @@
       <c r="BK41" s="28"/>
       <c r="BL41" s="28"/>
       <c r="BM41" s="28"/>
-      <c r="BN41" s="90"/>
-      <c r="BO41" s="91"/>
-      <c r="BP41" s="89"/>
+      <c r="BN41" s="89"/>
+      <c r="BO41" s="90"/>
+      <c r="BP41" s="88"/>
       <c r="BQ41" s="28"/>
       <c r="BR41" s="28"/>
     </row>
     <row r="42" spans="1:70" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="32"/>
       <c r="B42" s="47" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C42" s="41"/>
       <c r="D42" s="20">
@@ -5615,7 +5629,7 @@
         <v>44904</v>
       </c>
       <c r="G42" s="11">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="H42" s="28"/>
@@ -5676,9 +5690,9 @@
       <c r="BK42" s="28"/>
       <c r="BL42" s="28"/>
       <c r="BM42" s="28"/>
-      <c r="BN42" s="90"/>
-      <c r="BO42" s="91"/>
-      <c r="BP42" s="89"/>
+      <c r="BN42" s="89"/>
+      <c r="BO42" s="90"/>
+      <c r="BP42" s="88"/>
       <c r="BQ42" s="28"/>
       <c r="BR42" s="28"/>
     </row>
@@ -5748,9 +5762,9 @@
       <c r="BK43" s="28"/>
       <c r="BL43" s="28"/>
       <c r="BM43" s="28"/>
-      <c r="BN43" s="90"/>
-      <c r="BO43" s="91"/>
-      <c r="BP43" s="89"/>
+      <c r="BN43" s="89"/>
+      <c r="BO43" s="90"/>
+      <c r="BP43" s="88"/>
       <c r="BQ43" s="28"/>
       <c r="BR43" s="28"/>
     </row>
@@ -5758,15 +5772,13 @@
       <c r="A44" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="24" t="s">
-        <v>13</v>
-      </c>
+      <c r="B44" s="24"/>
       <c r="C44" s="25"/>
       <c r="D44" s="26"/>
       <c r="E44" s="53"/>
       <c r="F44" s="54"/>
       <c r="G44" s="27" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="H44" s="30"/>
@@ -5827,9 +5839,9 @@
       <c r="BK44" s="30"/>
       <c r="BL44" s="30"/>
       <c r="BM44" s="30"/>
-      <c r="BN44" s="93"/>
-      <c r="BO44" s="94"/>
-      <c r="BP44" s="92"/>
+      <c r="BN44" s="92"/>
+      <c r="BO44" s="93"/>
+      <c r="BP44" s="91"/>
       <c r="BQ44" s="30"/>
       <c r="BR44" s="30"/>
     </row>

</xml_diff>